<commit_message>
Change answer to Gov.CONTROL.01
</commit_message>
<xml_diff>
--- a/CISASAGReader-spreadsheet.xlsx
+++ b/CISASAGReader-spreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dick\ReliableEnergyAnalytics\PATENTS\SAG\SAGMVP\SAG-PM\OPEN-SOURCE\CISASAGReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3D2628-2C60-4BE2-9759-12E9750A4E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B79DA6-660E-4E0D-AB58-3CC64B232396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="729" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4610,6 +4610,10 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -4631,6 +4635,14 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -4757,18 +4769,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -6669,7 +6669,7 @@
   <dimension ref="A1:T57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="86" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35:P35"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -6698,31 +6698,31 @@
       <c r="J1" s="34"/>
       <c r="K1" s="34"/>
       <c r="L1" s="34"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
     </row>
     <row r="2" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="34"/>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
       <c r="Q2" s="34"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -6746,11 +6746,11 @@
     </row>
     <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="34"/>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
       <c r="E4" s="34"/>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
@@ -6768,22 +6768,22 @@
     <row r="5" spans="1:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="86" t="s">
         <v>931</v>
       </c>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="86"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86"/>
       <c r="Q5" s="34"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -6808,22 +6808,22 @@
     <row r="7" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="86" t="s">
         <v>886</v>
       </c>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="83"/>
-      <c r="N7" s="83"/>
-      <c r="O7" s="83"/>
-      <c r="P7" s="83"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
       <c r="Q7" s="34"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -6848,22 +6848,22 @@
     <row r="9" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
-      <c r="C9" s="83" t="s">
+      <c r="C9" s="86" t="s">
         <v>932</v>
       </c>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="83"/>
-      <c r="O9" s="83"/>
-      <c r="P9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
       <c r="Q9" s="34"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -6888,22 +6888,22 @@
     <row r="11" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34"/>
       <c r="B11" s="34"/>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="83"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="83"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="83"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="N11" s="83"/>
-      <c r="O11" s="83"/>
-      <c r="P11" s="83"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
       <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.3">
@@ -6988,11 +6988,11 @@
     </row>
     <row r="16" spans="1:17" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
       <c r="E16" s="34"/>
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
@@ -7010,135 +7010,135 @@
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="34"/>
       <c r="B17" s="34"/>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="76"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="71" t="s">
+      <c r="D17" s="79"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="72" t="s">
         <v>934</v>
       </c>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="72"/>
-      <c r="P17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="74"/>
       <c r="Q17" s="34"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="34"/>
       <c r="B18" s="34"/>
-      <c r="C18" s="78" t="s">
+      <c r="C18" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="79"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="71">
+      <c r="D18" s="82"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="72">
         <v>9786961788</v>
       </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="72"/>
-      <c r="O18" s="72"/>
-      <c r="P18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="74"/>
       <c r="Q18" s="34"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="34"/>
       <c r="B19" s="34"/>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="76"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="114">
-        <v>45633</v>
-      </c>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
-      <c r="N19" s="72"/>
-      <c r="O19" s="72"/>
-      <c r="P19" s="73"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="76">
+        <v>45658</v>
+      </c>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="73"/>
+      <c r="N19" s="73"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="74"/>
       <c r="Q19" s="34"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="34"/>
       <c r="B20" s="34"/>
-      <c r="C20" s="78" t="s">
+      <c r="C20" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="79"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="115" t="s">
+      <c r="D20" s="82"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="75" t="s">
         <v>935</v>
       </c>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="72"/>
-      <c r="O20" s="72"/>
-      <c r="P20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="74"/>
       <c r="Q20" s="34"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="34"/>
       <c r="B21" s="34"/>
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="76"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="72"/>
-      <c r="N21" s="72"/>
-      <c r="O21" s="72"/>
-      <c r="P21" s="73"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="73"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="74"/>
       <c r="Q21" s="34"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="34"/>
       <c r="B22" s="34"/>
-      <c r="C22" s="78" t="s">
+      <c r="C22" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
-      <c r="M22" s="72"/>
-      <c r="N22" s="72"/>
-      <c r="O22" s="72"/>
-      <c r="P22" s="73"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="73"/>
+      <c r="O22" s="73"/>
+      <c r="P22" s="74"/>
       <c r="Q22" s="34"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
@@ -7162,12 +7162,12 @@
     </row>
     <row r="24" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="34"/>
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
       <c r="F24" s="34"/>
       <c r="G24" s="34"/>
       <c r="H24" s="34"/>
@@ -7220,11 +7220,11 @@
       <c r="E26" s="60"/>
       <c r="F26" s="36">
         <f>COUNTIF(Governance!$C$13:$C$31, "=Yes")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G26" s="37">
         <f>COUNTIF(Governance!$C$13:$C$31, "=No")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26" s="37" t="s">
         <v>17</v>
@@ -7260,11 +7260,11 @@
       </c>
       <c r="H27" s="38">
         <f>SUM('Supply Chain'!J4+'Secure Development'!J4+'Secure Deployment'!J4+Vulnerability!J4)</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I27" s="63">
         <f>SUM('Supply Chain'!K4+'Secure Development'!K4+'Secure Deployment'!K4+Vulnerability!K4)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J27" s="63"/>
       <c r="K27" s="34"/>
@@ -7293,11 +7293,11 @@
       </c>
       <c r="H28" s="39">
         <f>SUM('Supply Chain'!J5+'Secure Development'!J5+'Secure Deployment'!J5+Vulnerability!J5)</f>
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I28" s="62">
         <f>SUM('Supply Chain'!K5+'Secure Development'!K5+'Secure Deployment'!K5+Vulnerability!K5)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="J28" s="62"/>
       <c r="K28" s="34"/>
@@ -7440,13 +7440,13 @@
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
-      <c r="C35" s="68" t="s">
+      <c r="C35" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="69"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="116">
-        <v>45633</v>
+      <c r="D35" s="70"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="68">
+        <v>45658</v>
       </c>
       <c r="G35" s="67"/>
       <c r="H35" s="67"/>
@@ -7624,10 +7624,10 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="12" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="12" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -7651,17 +7651,17 @@
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="99"/>
     </row>
     <row r="2" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="99"/>
       <c r="F2" t="s">
         <v>25</v>
       </c>
@@ -7670,9 +7670,9 @@
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="96"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="99"/>
       <c r="G3" t="s">
         <v>11</v>
       </c>
@@ -7693,19 +7693,19 @@
       <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="94"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="96"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="99"/>
       <c r="G4" t="s">
         <v>16</v>
       </c>
       <c r="H4">
         <f>COUNTIF($C$13:$C$31, "=Yes")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4">
         <f>COUNTIF($C$13:$C$31, "=No")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
@@ -7719,9 +7719,9 @@
       <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="96"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="99"/>
       <c r="G5" t="s">
         <v>18</v>
       </c>
@@ -7735,20 +7735,20 @@
       </c>
       <c r="J5">
         <f>SUM('Supply Chain'!J4+'Secure Development'!J4+'Secure Deployment'!J4+Vulnerability!J4)</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K5">
         <f>SUM('Supply Chain'!K4+'Secure Development'!K4+'Secure Deployment'!K4+Vulnerability!K4)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="93"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="96"/>
       <c r="G6" t="s">
         <v>26</v>
       </c>
@@ -7762,37 +7762,37 @@
       </c>
       <c r="J6">
         <f>SUM('Supply Chain'!J5+'Secure Development'!J5+'Secure Deployment'!J5+Vulnerability!J5)</f>
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="K6">
         <f>SUM('Supply Chain'!K5+'Secure Development'!K5+'Secure Deployment'!K5+Vulnerability!K5)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="87" t="s">
+      <c r="B7" s="90" t="s">
         <v>923</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="84"/>
-      <c r="B8" s="89"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
+      <c r="A8" s="87"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
     </row>
     <row r="9" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="85"/>
-      <c r="B9" s="89"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
+      <c r="A9" s="88"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="20"/>
@@ -7827,7 +7827,7 @@
         <v>927</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>33</v>
@@ -8182,27 +8182,27 @@
       <c r="A1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="105" t="s">
         <v>919</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="104"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="107"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="105"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="107"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="110"/>
       <c r="I3" t="s">
         <v>66</v>
       </c>
@@ -8226,10 +8226,10 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="108"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="110"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="113"/>
       <c r="H4" t="s">
         <v>18</v>
       </c>
@@ -8263,12 +8263,12 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="105" t="s">
         <v>922</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="104"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="107"/>
       <c r="H5" t="s">
         <v>68</v>
       </c>
@@ -8300,56 +8300,56 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="105"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="107"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="110"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="108"/>
-      <c r="C7" s="109"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="110"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="113"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="105" t="s">
         <v>920</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="104"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="107"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="108"/>
-      <c r="C9" s="109"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="110"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="113"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="113"/>
+      <c r="C10" s="115"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="116"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" s="20"/>
       <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="99" t="s">
+      <c r="B12" s="102" t="s">
         <v>921</v>
       </c>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="104"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="99"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="101"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="104"/>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23"/>
@@ -9552,8 +9552,8 @@
   </sheetPr>
   <dimension ref="A1:O229"/>
   <sheetViews>
-    <sheetView topLeftCell="A229" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView topLeftCell="A117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -9575,27 +9575,27 @@
       <c r="A1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="105" t="s">
         <v>919</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="104"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="107"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="105"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="107"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="110"/>
       <c r="I3" t="s">
         <v>66</v>
       </c>
@@ -9619,10 +9619,10 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="108"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="110"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="113"/>
       <c r="H4" t="s">
         <v>18</v>
       </c>
@@ -9632,11 +9632,11 @@
       </c>
       <c r="J4">
         <f>COUNTIFS($A$16:$A$228, "=CONTROL.DEV.*", $E16:$E228, "*skip*")</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K4">
         <f>I4-(J4+SUM(L4:O4))</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L4">
         <f>COUNTIFS($A$16:$A$228, "=CONTROL.DEV.*",$C$16:$C$228, "=Yes")</f>
@@ -9656,12 +9656,12 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="105" t="s">
         <v>922</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="104"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="107"/>
       <c r="H5" t="s">
         <v>68</v>
       </c>
@@ -9671,11 +9671,11 @@
       </c>
       <c r="J5">
         <f>COUNTIFS($A$16:$A$300, "=TASK.dev.*", $E$16:$E$300, "*skip*")</f>
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K5">
         <f>I5-(J5+SUM(L5:O5))</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L5">
         <f>COUNTIFS($A$16:$A$300, "=TASK.DEV.*",$C$16:$C$300, "=Yes")</f>
@@ -9693,56 +9693,56 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="105"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="107"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="110"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="108"/>
-      <c r="C7" s="109"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="110"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="113"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="105" t="s">
         <v>920</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="104"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="107"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="108"/>
-      <c r="C9" s="109"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="110"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="113"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="113"/>
+      <c r="C10" s="115"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="116"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" s="20"/>
       <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="99" t="s">
+      <c r="B12" s="102" t="s">
         <v>921</v>
       </c>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="104"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="99"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="101"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="104"/>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23"/>
@@ -11650,11 +11650,11 @@
       </c>
       <c r="D120" s="10" t="str">
         <f>IF(E120 = "You May Skip This Question Because You Answered the Associated Governance Question Yes","Move to Next CONTROL Question.",IF(ISBLANK(C120),"Select Answer to CONTROL Question from Drop Down List", IF(C120 = "Partial","Answer Associated TASK Questions", "Review Any Remaining Unanswered CONTROL Questions")))</f>
-        <v>Answer Associated TASK Questions</v>
+        <v>Move to Next CONTROL Question.</v>
       </c>
       <c r="E120" s="12" t="str">
         <f>IF(ISBLANK(Governance!$C$13), "Please Complete this Question", IF(Governance!$C$13 = "Yes", "You May Skip This Question Because You Answered the Associated Governance Question Yes", IF(ISBLANK($C$120),"Please Complete this Question","Continue with Next Indicated Question")))</f>
-        <v>Continue with Next Indicated Question</v>
+        <v>You May Skip This Question Because You Answered the Associated Governance Question Yes</v>
       </c>
       <c r="G120" t="s">
         <v>296</v>
@@ -11675,11 +11675,11 @@
       </c>
       <c r="D121" s="8" t="str">
         <f t="shared" si="14"/>
-        <v>Move to Next Question</v>
+        <v>Question skipped</v>
       </c>
       <c r="E121" s="29" t="str">
         <f>IF(ISNUMBER(SEARCH("skip", $E$120)), "Task question skipped due to Governance response", IF(ISBLANK($C$120),"Please Complete the Associated CONTROL Question",IF(OR($C$120="Yes", $C$120="No", $C$120="N/A"),"You May Skip This Question Because You Answered the Associated CONTROL Question","Please Complete this Question")))</f>
-        <v>Please Complete this Question</v>
+        <v>Task question skipped due to Governance response</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="60" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -11694,11 +11694,11 @@
       </c>
       <c r="D122" s="8" t="str">
         <f t="shared" si="14"/>
-        <v>Move to Next Question</v>
+        <v>Question skipped</v>
       </c>
       <c r="E122" s="29" t="str">
         <f t="shared" ref="E122:E123" si="16">IF(ISNUMBER(SEARCH("skip", $E$120)), "Task question skipped due to Governance response", IF(ISBLANK($C$120),"Please Complete the Associated CONTROL Question",IF(OR($C$120="Yes", $C$120="No", $C$120="N/A"),"You May Skip This Question Because You Answered the Associated CONTROL Question","Please Complete this Question")))</f>
-        <v>Please Complete this Question</v>
+        <v>Task question skipped due to Governance response</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="60" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -11713,11 +11713,11 @@
       </c>
       <c r="D123" s="8" t="str">
         <f t="shared" si="14"/>
-        <v>Move to Next Question</v>
+        <v>Question skipped</v>
       </c>
       <c r="E123" s="29" t="str">
         <f t="shared" si="16"/>
-        <v>Please Complete this Question</v>
+        <v>Task question skipped due to Governance response</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -13908,27 +13908,27 @@
       <c r="A1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="105" t="s">
         <v>919</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="104"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="107"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="105"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="107"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="110"/>
       <c r="I3" t="s">
         <v>66</v>
       </c>
@@ -13952,10 +13952,10 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="108"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="110"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="113"/>
       <c r="H4" t="s">
         <v>18</v>
       </c>
@@ -13989,12 +13989,12 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="105" t="s">
         <v>922</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="104"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="107"/>
       <c r="H5" t="s">
         <v>68</v>
       </c>
@@ -14026,56 +14026,56 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="105"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="107"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="110"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="108"/>
-      <c r="C7" s="109"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="110"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="113"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="105" t="s">
         <v>920</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="104"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="107"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="108"/>
-      <c r="C9" s="109"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="110"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="113"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="113"/>
+      <c r="C10" s="115"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="116"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" s="20"/>
       <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="99" t="s">
+      <c r="B12" s="102" t="s">
         <v>921</v>
       </c>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="104"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="99"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="101"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="104"/>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23"/>
@@ -15533,27 +15533,27 @@
       <c r="A1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="105" t="s">
         <v>919</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="104"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="107"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="105"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="107"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="110"/>
       <c r="I3" t="s">
         <v>66</v>
       </c>
@@ -15577,10 +15577,10 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="108"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="110"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="113"/>
       <c r="H4" t="s">
         <v>18</v>
       </c>
@@ -15614,12 +15614,12 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="105" t="s">
         <v>922</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="104"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="107"/>
       <c r="H5" t="s">
         <v>68</v>
       </c>
@@ -15651,56 +15651,56 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="105"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="107"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="110"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="108"/>
-      <c r="C7" s="109"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="110"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="113"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="105" t="s">
         <v>920</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="104"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="107"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="108"/>
-      <c r="C9" s="109"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="110"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="113"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="113"/>
+      <c r="C10" s="115"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="116"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" s="20"/>
       <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="99" t="s">
+      <c r="B12" s="102" t="s">
         <v>921</v>
       </c>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="104"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="99"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="101"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="104"/>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23"/>

</xml_diff>